<commit_message>
merge with develop branch
</commit_message>
<xml_diff>
--- a/docs/write-pair.xlsx
+++ b/docs/write-pair.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420"/>
+    <workbookView windowWidth="21540" windowHeight="11115"/>
   </bookViews>
   <sheets>
     <sheet name="key2copy" sheetId="1" r:id="rId1"/>
@@ -400,9 +400,337 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ProposedInEpochPrefix </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>= []</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF002FA6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"proposed-in-epoch-"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">StartMarkProposalInEpochPrefix </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>= []</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF002FA6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"sp-in-epoch-"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>schema.go</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">databaseVerisionKey </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>= []</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF002FA6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"DatabaseVersion"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">headHeaderKey </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>= []</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF002FA6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"LastHeader"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">headBlockKey </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>= []</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF002FA6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"LastBlock"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>headFastBlockKey = []byte("LastFast")</t>
+  </si>
+  <si>
+    <t>fastTrieProgressKey = []byte("TrieSync")</t>
+  </si>
+  <si>
+    <t>done in raw copy(block related)</t>
+  </si>
+  <si>
+    <t>headerPrefix       = []byte("h") // headerPrefix + num (uint64 big endian) + hash -&gt; header</t>
+  </si>
+  <si>
+    <t>headerTDSuffix     = []byte("t") // headerPrefix + num (uint64 big endian) + hash + headerTDSuffix -&gt; td</t>
+  </si>
+  <si>
+    <t>headerHashSuffix   = []byte("n") // headerPrefix + num (uint64 big endian) + headerHashSuffix -&gt; hash</t>
+  </si>
+  <si>
+    <t>headerNumberPrefix = []byte("H") // headerNumberPrefix + hash -&gt; num (uint64 big endian)</t>
+  </si>
+  <si>
+    <t>blockBodyPrefix     = []byte("b") // blockBodyPrefix + num (uint64 big endian) + hash -&gt; block body</t>
+  </si>
+  <si>
     <t>not copy this time</t>
   </si>
   <si>
+    <t>blockReceiptsPrefix = []byte("r") // blockReceiptsPrefix + num (uint64 big endian) + hash -&gt; block receipts</t>
+  </si>
+  <si>
+    <t>txLookupPrefix  = []byte("l") // txLookupPrefix + hash -&gt; transaction/receipt lookup metadata</t>
+  </si>
+  <si>
+    <t>bloomBitsPrefix = []byte("B") // bloomBitsPrefix + bit (uint16 big endian) + section (uint64 big endian) + hash -&gt; bloom bits</t>
+  </si>
+  <si>
+    <t>preimagePrefix = []byte("secure-key-")      // preimagePrefix + hash -&gt; preimage</t>
+  </si>
+  <si>
+    <t>configPrefix   = []byte("ethereum-config-") // config prefix for the db</t>
+  </si>
+  <si>
+    <t>BloomBitsIndexPrefix = []byte("iB") // BloomBitsIndexPrefix is the data table of a chain indexer to track its progress</t>
+  </si>
+  <si>
+    <t>database.go</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10.5"/>
@@ -410,7 +738,7 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">ProposedInEpochPrefix </t>
+      <t xml:space="preserve">secureKeyPrefix </t>
     </r>
     <r>
       <rPr>
@@ -446,7 +774,7 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>"proposed-in-epoch-"</t>
+      <t>"secure-key-"</t>
     </r>
     <r>
       <rPr>
@@ -459,6 +787,30 @@
     </r>
   </si>
   <si>
+    <t>//in "prunedata" db, will not snapshot, no need to copy</t>
+  </si>
+  <si>
+    <t>schema_data_prune.go</t>
+  </si>
+  <si>
+    <t>headDataScanKey = []byte("LastDataScanHeight")</t>
+  </si>
+  <si>
+    <t>headDataPruneKey = []byte("LastDataPruneHeight")</t>
+  </si>
+  <si>
+    <t>dataPruneProcessPrefix = []byte("p") // dataPruneProcessPrefix + scan num (uint64 big endian) + prune num (uint64 big endian) + dataPruneProcessSuffix -&gt; trie root hash</t>
+  </si>
+  <si>
+    <t>dataPruneProcessSuffix = []byte("n")</t>
+  </si>
+  <si>
+    <t>//in "tx3cache" db, will not snapshot, no need to copy</t>
+  </si>
+  <si>
+    <t>tx3_local_database_util.go</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10.5"/>
@@ -466,7 +818,7 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">StartMarkProposalInEpochPrefix </t>
+      <t xml:space="preserve">tx3Prefix       </t>
     </r>
     <r>
       <rPr>
@@ -502,20 +854,27 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>"sp-in-epoch-"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>schema.go</t>
+      <t>"t"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color rgb="FF8C8C8C"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>// tx3Prefix + chainId + txHash -&gt; tx3</t>
+    </r>
   </si>
   <si>
     <r>
@@ -525,7 +884,7 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">databaseVerisionKey </t>
+      <t xml:space="preserve">tx3LookupPrefix </t>
     </r>
     <r>
       <rPr>
@@ -561,16 +920,26 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>"DatabaseVersion"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>)</t>
+      <t>"k"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF121314"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color rgb="FF8C8C8C"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>// tx3LookupPrefix + chainId + txHash -&gt; tx3 lookup metadata</t>
     </r>
   </si>
   <si>
@@ -581,369 +950,6 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">headHeaderKey </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>= []</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF002FA6"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>byte</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>"LastHeader"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">headBlockKey </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>= []</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF002FA6"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>byte</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>"LastBlock"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>headFastBlockKey = []byte("LastFast")</t>
-  </si>
-  <si>
-    <t>fastTrieProgressKey = []byte("TrieSync")</t>
-  </si>
-  <si>
-    <t>done in raw copy(block related)</t>
-  </si>
-  <si>
-    <t>headerPrefix       = []byte("h") // headerPrefix + num (uint64 big endian) + hash -&gt; header</t>
-  </si>
-  <si>
-    <t>headerTDSuffix     = []byte("t") // headerPrefix + num (uint64 big endian) + hash + headerTDSuffix -&gt; td</t>
-  </si>
-  <si>
-    <t>headerHashSuffix   = []byte("n") // headerPrefix + num (uint64 big endian) + headerHashSuffix -&gt; hash</t>
-  </si>
-  <si>
-    <t>headerNumberPrefix = []byte("H") // headerNumberPrefix + hash -&gt; num (uint64 big endian)</t>
-  </si>
-  <si>
-    <t>blockBodyPrefix     = []byte("b") // blockBodyPrefix + num (uint64 big endian) + hash -&gt; block body</t>
-  </si>
-  <si>
-    <t>blockReceiptsPrefix = []byte("r") // blockReceiptsPrefix + num (uint64 big endian) + hash -&gt; block receipts</t>
-  </si>
-  <si>
-    <t>txLookupPrefix  = []byte("l") // txLookupPrefix + hash -&gt; transaction/receipt lookup metadata</t>
-  </si>
-  <si>
-    <t>bloomBitsPrefix = []byte("B") // bloomBitsPrefix + bit (uint16 big endian) + section (uint64 big endian) + hash -&gt; bloom bits</t>
-  </si>
-  <si>
-    <t>preimagePrefix = []byte("secure-key-")      // preimagePrefix + hash -&gt; preimage</t>
-  </si>
-  <si>
-    <t>configPrefix   = []byte("ethereum-config-") // config prefix for the db</t>
-  </si>
-  <si>
-    <t>BloomBitsIndexPrefix = []byte("iB") // BloomBitsIndexPrefix is the data table of a chain indexer to track its progress</t>
-  </si>
-  <si>
-    <t>database.go</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">secureKeyPrefix </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>= []</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF002FA6"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>byte</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>"secure-key-"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>//in "prunedata" db, will not snapshot, no need to copy</t>
-  </si>
-  <si>
-    <t>schema_data_prune.go</t>
-  </si>
-  <si>
-    <t>headDataScanKey = []byte("LastDataScanHeight")</t>
-  </si>
-  <si>
-    <t>headDataPruneKey = []byte("LastDataPruneHeight")</t>
-  </si>
-  <si>
-    <t>dataPruneProcessPrefix = []byte("p") // dataPruneProcessPrefix + scan num (uint64 big endian) + prune num (uint64 big endian) + dataPruneProcessSuffix -&gt; trie root hash</t>
-  </si>
-  <si>
-    <t>dataPruneProcessSuffix = []byte("n")</t>
-  </si>
-  <si>
-    <t>//in "tx3cache" db, will not snapshot, no need to copy</t>
-  </si>
-  <si>
-    <t>tx3_local_database_util.go</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">tx3Prefix       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>= []</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF002FA6"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>byte</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>"t"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10.5"/>
-        <color rgb="FF8C8C8C"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>// tx3Prefix + chainId + txHash -&gt; tx3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">tx3LookupPrefix </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>= []</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF002FA6"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>byte</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>"k"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF121314"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10.5"/>
-        <color rgb="FF8C8C8C"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>// tx3LookupPrefix + chainId + txHash -&gt; tx3 lookup metadata</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Tx3ProofPrefix  </t>
     </r>
     <r>
@@ -1008,10 +1014,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1078,6 +1084,82 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1087,14 +1169,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1108,29 +1198,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1145,22 +1221,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1168,60 +1228,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color rgb="FF121314"/>
       <name val="Consolas"/>
@@ -1243,13 +1249,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1261,121 +1375,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1388,42 +1430,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1434,6 +1440,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1501,186 +1540,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1721,54 +1727,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2073,14 +2079,14 @@
   <sheetPr/>
   <dimension ref="A3:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="46.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="45.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="46.8916666666667" customWidth="1"/>
+    <col min="2" max="2" width="45.775" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" s="6" customFormat="1" spans="2:2">
@@ -2156,23 +2162,23 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2180,7 +2186,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2188,7 +2194,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2196,7 +2202,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2204,7 +2210,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2212,52 +2218,52 @@
         <v>8</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>27</v>
@@ -2265,7 +2271,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>28</v>
@@ -2273,7 +2279,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>29</v>
@@ -2297,7 +2303,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>32</v>
@@ -2405,10 +2411,10 @@
       <selection activeCell="B4" sqref="B4:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
-    <col min="4" max="4" width="42.2222222222222" customWidth="1"/>
-    <col min="5" max="5" width="7.55555555555556" customWidth="1"/>
+    <col min="4" max="4" width="42.225" customWidth="1"/>
+    <col min="5" max="5" width="7.55833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6">
@@ -2439,7 +2445,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>